<commit_message>
Time out games test approvment
</commit_message>
<xml_diff>
--- a/CasinoGamesAPITest/CasinoGamesAPITest/src/test/java/timeOutGames/1CraftbetDataTimeOutGamesList.xlsx
+++ b/CasinoGamesAPITest/CasinoGamesAPITest/src/test/java/timeOutGames/1CraftbetDataTimeOutGamesList.xlsx
@@ -12,9 +12,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>3693263   LoL Pro League   Top Esports (LOL)  VS  JD Gaming (LOL)   E-sports   2022-08-26T13:00:00  Status = 1   After game start time out = :  4 hours  33 minutes</t>
+    <t>3708960   UruguaySegundaBNacional   Deportivo Colonia  VS  Club Oriental   Soccer   2022-08-27T22:48:33  Status = 1   After game start time out = :  16 hours  11 minutes</t>
+  </si>
+  <si>
+    <t>3708111   ITFW60Prerov   Irene Burillo Escorihuela  VS  Sada Nahimana   Tennis   2022-08-27T16:30:47  Status = 1   After game start time out = :  22 hours  29 minutes</t>
+  </si>
+  <si>
+    <t>3704769   ITF-M Celje   Roko Horvat  VS  Daniele Capecchi   Tennis   2022-08-27T18:00:00  Status = 1   After game start time out = :  21 hours  0 minutes</t>
+  </si>
+  <si>
+    <t>3709022   NFLPreseason   JAX Jaguars  VS  ATL Falcons   American Football   2022-08-27T22:58:53  Status = 1   After game start time out = :  16 hours  1 minutes</t>
+  </si>
+  <si>
+    <t>3708393   World Championships Women   Akane Yamaguchi  VS  CHEN Yu Fei   Badminton   2022-08-28T12:00:00  Status = 1   After game start time out = :  2 hours  59 minutes</t>
+  </si>
+  <si>
+    <t>3709018   MLB   LA Angels  VS  TOR Blue Jays   Baseball   2022-08-27T22:54:31  Status = 1   After game start time out = :  16 hours  5 minutes</t>
+  </si>
+  <si>
+    <t>3696193   European Championships Women   Hungary (W)  VS  Greece (W)   Water Polo   2022-08-27T22:30:00  Status = 1   After game start time out = :  16 hours  30 minutes</t>
+  </si>
+  <si>
+    <t>3708552   Curragh   4.15 Curragh (Race 6)  VS  ~N/A~   Horse Racing   2022-08-27T18:45:09  Status = 1   After game start time out = :  20 hours  15 minutes</t>
+  </si>
+  <si>
+    <t>3709013   SanIsidro   8.15 San Isidro (Race 7)  VS  ~N/A~   Horse Racing   2022-08-27T22:50:04  Status = 1   After game start time out = :  16 hours  10 minutes</t>
+  </si>
+  <si>
+    <t>3709037   EllisPark   Race 4 Ellis Park  VS  ~N/A~   Horse Racing   2022-08-27T23:05:03  Status = 1   After game start time out = :  15 hours  55 minutes</t>
   </si>
 </sst>
 </file>
@@ -59,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -73,6 +100,51 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>